<commit_message>
Add generated test cases from Claude
</commit_message>
<xml_diff>
--- a/Generated_TestCases.xlsx
+++ b/Generated_TestCases.xlsx
@@ -10125,7 +10125,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:H2"/>
@@ -10247,161 +10247,698 @@
       <c r="I5" s="53" t="n"/>
     </row>
     <row r="6" ht="99.75" customHeight="1">
-      <c r="B6" s="57" t="n"/>
-      <c r="C6" s="60" t="n"/>
-      <c r="D6" s="70" t="n"/>
-      <c r="E6" s="61" t="n"/>
-      <c r="F6" s="62" t="n"/>
-      <c r="G6" s="58" t="inlineStr">
-        <is>
-          <t>Not Executed</t>
-        </is>
-      </c>
-      <c r="H6" s="59" t="n"/>
+      <c r="B6" s="57" t="inlineStr">
+        <is>
+          <t>F001</t>
+        </is>
+      </c>
+      <c r="C6" s="60" t="inlineStr">
+        <is>
+          <t>Application is installed and launched</t>
+        </is>
+      </c>
+      <c r="D6" s="70" t="inlineStr">
+        <is>
+          <t>Network Packet Capture - Start</t>
+        </is>
+      </c>
+      <c r="E6" s="61" t="inlineStr">
+        <is>
+          <t>1. Navigate to Network Packet Capture section&lt;br&gt;2. Click on Start button</t>
+        </is>
+      </c>
+      <c r="F6" s="62" t="inlineStr">
+        <is>
+          <t>Packet capture starts successfully</t>
+        </is>
+      </c>
+      <c r="G6" s="58" t="inlineStr"/>
+      <c r="H6" s="59" t="inlineStr"/>
       <c r="I6" s="53" t="n"/>
     </row>
     <row r="7" ht="99.75" customHeight="1">
-      <c r="B7" s="57" t="n"/>
-      <c r="C7" s="60" t="n"/>
-      <c r="D7" s="70" t="n"/>
-      <c r="E7" s="61" t="n"/>
-      <c r="F7" s="62" t="n"/>
-      <c r="G7" s="58" t="inlineStr">
-        <is>
-          <t>Not Executed</t>
-        </is>
-      </c>
-      <c r="H7" s="59" t="n"/>
+      <c r="B7" s="57" t="inlineStr">
+        <is>
+          <t>F002</t>
+        </is>
+      </c>
+      <c r="C7" s="60" t="inlineStr">
+        <is>
+          <t>Packet capture is in progress</t>
+        </is>
+      </c>
+      <c r="D7" s="70" t="inlineStr">
+        <is>
+          <t>Network Packet Capture - Stop</t>
+        </is>
+      </c>
+      <c r="E7" s="61" t="inlineStr">
+        <is>
+          <t>1. Navigate to Network Packet Capture section&lt;br&gt;2. Click on Stop button</t>
+        </is>
+      </c>
+      <c r="F7" s="62" t="inlineStr">
+        <is>
+          <t>1. Packet capture stops&lt;br&gt;2. .pcap file is generated&lt;br&gt;3. File is copied to MFP's Shared Folder&lt;br&gt;4. Shared Folder opens automatically</t>
+        </is>
+      </c>
+      <c r="G7" s="58" t="inlineStr"/>
+      <c r="H7" s="59" t="inlineStr"/>
       <c r="I7" s="53" t="n"/>
     </row>
     <row r="8" ht="99.75" customHeight="1">
-      <c r="B8" s="57" t="n"/>
-      <c r="C8" s="60" t="n"/>
-      <c r="D8" s="70" t="n"/>
-      <c r="E8" s="61" t="n"/>
-      <c r="F8" s="62" t="n"/>
-      <c r="G8" s="58" t="inlineStr">
-        <is>
-          <t>Not Executed</t>
-        </is>
-      </c>
-      <c r="H8" s="59" t="n"/>
+      <c r="B8" s="57" t="inlineStr">
+        <is>
+          <t>F003</t>
+        </is>
+      </c>
+      <c r="C8" s="60" t="inlineStr">
+        <is>
+          <t>Application is installed and launched</t>
+        </is>
+      </c>
+      <c r="D8" s="70" t="inlineStr">
+        <is>
+          <t>Memory Leak Check - Table Display</t>
+        </is>
+      </c>
+      <c r="E8" s="61" t="inlineStr">
+        <is>
+          <t>1. Navigate to Memory Leak Check section</t>
+        </is>
+      </c>
+      <c r="F8" s="62" t="inlineStr">
+        <is>
+          <t>Protocol-specific Memory Leak Comparison Table is displayed</t>
+        </is>
+      </c>
+      <c r="G8" s="58" t="inlineStr"/>
+      <c r="H8" s="59" t="inlineStr"/>
       <c r="I8" s="53" t="n"/>
     </row>
     <row r="9" ht="99.75" customHeight="1">
-      <c r="B9" s="57" t="n"/>
-      <c r="C9" s="60" t="n"/>
-      <c r="D9" s="70" t="n"/>
-      <c r="E9" s="61" t="n"/>
-      <c r="F9" s="62" t="n"/>
-      <c r="G9" s="58" t="inlineStr">
-        <is>
-          <t>Not Executed</t>
-        </is>
-      </c>
-      <c r="H9" s="59" t="n"/>
+      <c r="B9" s="57" t="inlineStr">
+        <is>
+          <t>F004</t>
+        </is>
+      </c>
+      <c r="C9" s="60" t="inlineStr">
+        <is>
+          <t>Memory Leak Check section is open</t>
+        </is>
+      </c>
+      <c r="D9" s="70" t="inlineStr">
+        <is>
+          <t>Memory Leak Check - Comparison</t>
+        </is>
+      </c>
+      <c r="E9" s="61" t="inlineStr">
+        <is>
+          <t>1. Review the Memory Leak Comparison Table&lt;br&gt;2. Compare values to determine memory leak</t>
+        </is>
+      </c>
+      <c r="F9" s="62" t="inlineStr">
+        <is>
+          <t>User can easily determine if a memory leak has occurred based on the comparison table</t>
+        </is>
+      </c>
+      <c r="G9" s="58" t="inlineStr"/>
+      <c r="H9" s="59" t="inlineStr"/>
       <c r="I9" s="53" t="n"/>
     </row>
     <row r="10" ht="99.75" customHeight="1">
-      <c r="B10" s="57" t="n"/>
-      <c r="C10" s="60" t="n"/>
-      <c r="D10" s="70" t="n"/>
-      <c r="E10" s="61" t="n"/>
-      <c r="F10" s="62" t="n"/>
-      <c r="G10" s="58" t="inlineStr">
-        <is>
-          <t>Not Executed</t>
-        </is>
-      </c>
-      <c r="H10" s="59" t="n"/>
+      <c r="B10" s="57" t="inlineStr">
+        <is>
+          <t>F005</t>
+        </is>
+      </c>
+      <c r="C10" s="60" t="inlineStr">
+        <is>
+          <t>Application is installed and launched</t>
+        </is>
+      </c>
+      <c r="D10" s="70" t="inlineStr">
+        <is>
+          <t>Debug Log Collection</t>
+        </is>
+      </c>
+      <c r="E10" s="61" t="inlineStr">
+        <is>
+          <t>1. Navigate to Debug Log Collection section&lt;br&gt;2. Click on Run button</t>
+        </is>
+      </c>
+      <c r="F10" s="62" t="inlineStr">
+        <is>
+          <t>1. Script executes successfully&lt;br&gt;2. Logs are collected&lt;br&gt;3. Logs are copied to MFP's Shared Folder&lt;br&gt;4. Shared Folder opens automatically</t>
+        </is>
+      </c>
+      <c r="G10" s="58" t="inlineStr"/>
+      <c r="H10" s="59" t="inlineStr"/>
       <c r="I10" s="53" t="n"/>
     </row>
     <row r="11" ht="99.75" customHeight="1">
-      <c r="B11" s="57" t="n"/>
-      <c r="C11" s="60" t="n"/>
-      <c r="D11" s="70" t="n"/>
-      <c r="E11" s="61" t="n"/>
-      <c r="F11" s="62" t="n"/>
-      <c r="G11" s="58" t="inlineStr">
-        <is>
-          <t>Not Executed</t>
-        </is>
-      </c>
-      <c r="H11" s="59" t="n"/>
+      <c r="B11" s="57" t="inlineStr">
+        <is>
+          <t>F006</t>
+        </is>
+      </c>
+      <c r="C11" s="60" t="inlineStr">
+        <is>
+          <t>Debug Log Collection failed on first attempt</t>
+        </is>
+      </c>
+      <c r="D11" s="70" t="inlineStr">
+        <is>
+          <t>Debug Log Collection - Retry</t>
+        </is>
+      </c>
+      <c r="E11" s="61" t="inlineStr">
+        <is>
+          <t>1. Navigate to Debug Log Collection section&lt;br&gt;2. Click on Run button again</t>
+        </is>
+      </c>
+      <c r="F11" s="62" t="inlineStr">
+        <is>
+          <t>1. Script executes successfully&lt;br&gt;2. Logs are collected&lt;br&gt;3. Logs are copied to MFP's Shared Folder&lt;br&gt;4. Shared Folder opens with logs visible</t>
+        </is>
+      </c>
+      <c r="G11" s="58" t="inlineStr"/>
+      <c r="H11" s="59" t="inlineStr"/>
       <c r="I11" s="53" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="63" t="n"/>
-      <c r="B12" s="63" t="n"/>
-      <c r="C12" s="63" t="n"/>
-      <c r="D12" s="63" t="n"/>
-      <c r="E12" s="64" t="n"/>
-      <c r="F12" s="64" t="n"/>
-      <c r="G12" s="63" t="n"/>
-      <c r="H12" s="63" t="n"/>
+      <c r="B12" s="63" t="inlineStr">
+        <is>
+          <t>F007</t>
+        </is>
+      </c>
+      <c r="C12" s="63" t="inlineStr">
+        <is>
+          <t>Application is installed and launched</t>
+        </is>
+      </c>
+      <c r="D12" s="63" t="inlineStr">
+        <is>
+          <t>Diagnostic Code Details - ECC</t>
+        </is>
+      </c>
+      <c r="E12" s="64" t="inlineStr">
+        <is>
+          <t>1. Navigate to Diagnostic Code Details section&lt;br&gt;2. Select ECC option</t>
+        </is>
+      </c>
+      <c r="F12" s="64" t="inlineStr">
+        <is>
+          <t>Relevant job-specific details for ECC are displayed</t>
+        </is>
+      </c>
+      <c r="G12" s="63" t="inlineStr"/>
+      <c r="H12" s="63" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>F008</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Application is installed and launched</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Diagnostic Code Details - Network Protocols</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1. Navigate to Diagnostic Code Details section&lt;br&gt;2. Select Network Protocols option</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Relevant job-specific details for Network Protocols are displayed</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="B14" s="45" t="inlineStr">
         <is>
-          <t>Test Summary</t>
-        </is>
-      </c>
-      <c r="C14" s="67" t="n"/>
+          <t>F009</t>
+        </is>
+      </c>
+      <c r="C14" s="67" t="inlineStr">
+        <is>
+          <t>Application is installed and launched</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Diagnostic Code Details - High Security Mode</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1. Navigate to Diagnostic Code Details section&lt;br&gt;2. Select High Security Mode option</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Relevant job-specific details for High Security Mode are displayed</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
     </row>
     <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>F010</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Application is installed and launched</t>
+        </is>
+      </c>
       <c r="D15" s="45" t="inlineStr">
         <is>
-          <t>Test Case Count:</t>
-        </is>
-      </c>
+          <t>Diagnostic Code Details - Common Codes</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>1. Navigate to Diagnostic Code Details section&lt;br&gt;2. Select commonly used diagnostic codes</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Relevant job-specific details for selected diagnostic codes are displayed</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>F011</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Application is installed and launched</t>
+        </is>
+      </c>
       <c r="D16" s="46" t="inlineStr">
         <is>
-          <t>Total Test Cases</t>
-        </is>
-      </c>
-      <c r="E16" s="71">
-        <f>COUNTA(B6:B6)</f>
-        <v/>
-      </c>
+          <t>08 Diagnostic Code Value - Get</t>
+        </is>
+      </c>
+      <c r="E16" s="71" t="inlineStr">
+        <is>
+          <t>1. Navigate to 08 Diagnostic Code Value section&lt;br&gt;2. Select a diagnostic code&lt;br&gt;3. Click on Get button</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Current value of the selected diagnostic code is displayed</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
     </row>
     <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>F012</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Application is installed and launched</t>
+        </is>
+      </c>
       <c r="D17" s="65" t="inlineStr">
         <is>
-          <t>Total Test Case Passed</t>
-        </is>
-      </c>
-      <c r="E17" s="71">
-        <f>COUNTIF(G6:G6,"PASS")</f>
-        <v/>
-      </c>
+          <t>08 Diagnostic Code Value - Set</t>
+        </is>
+      </c>
+      <c r="E17" s="71" t="inlineStr">
+        <is>
+          <t>1. Navigate to 08 Diagnostic Code Value section&lt;br&gt;2. Select a diagnostic code&lt;br&gt;3. Enter a new value&lt;br&gt;4. Click on Set button</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>The diagnostic code value is updated successfully</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
     </row>
     <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>F013</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Application is installed and launched</t>
+        </is>
+      </c>
       <c r="D18" s="46" t="inlineStr">
         <is>
-          <t>Total Test Case Failed</t>
-        </is>
-      </c>
-      <c r="E18" s="71">
-        <f>COUNTIF(G6:G6,"FAIL")</f>
-        <v/>
-      </c>
+          <t>Protocol Configuration - Get</t>
+        </is>
+      </c>
+      <c r="E18" s="71" t="inlineStr">
+        <is>
+          <t>1. Navigate to Protocol Configuration section&lt;br&gt;2. Open Protocol Selection Window&lt;br&gt;3. Select a protocol&lt;br&gt;4. Click on Get button</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Current value of the selected protocol is displayed</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
     </row>
     <row r="19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>F014</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Application is installed and launched</t>
+        </is>
+      </c>
       <c r="D19" s="68" t="inlineStr">
         <is>
-          <t>Total Test Case Not  Executed</t>
-        </is>
-      </c>
-      <c r="E19" s="71">
-        <f>COUNTIF(G6:G6,"Not Executed")</f>
-        <v/>
+          <t>Protocol Configuration - Set (Pending)</t>
+        </is>
+      </c>
+      <c r="E19" s="71" t="inlineStr">
+        <is>
+          <t>1. Navigate to Protocol Configuration section&lt;br&gt;2. Open Protocol Selection Window&lt;br&gt;3. Select a protocol&lt;br&gt;4. Enter a new value&lt;br&gt;5. Click on Set button</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Feature is marked as "Not Implemented" or similar message is displayed</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Feature pending implementation as per SRS</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Test Case ID</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Preconditions</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Test Condition</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Steps with description</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Expected Result</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Actual Result</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Remarks</t>
+        </is>
       </c>
     </row>
     <row r="21">
-      <c r="D21" s="45" t="n"/>
-      <c r="E21" s="69" t="n"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>--------------</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>---------------</t>
+        </is>
+      </c>
+      <c r="D21" s="45" t="inlineStr">
+        <is>
+          <t>----------------</t>
+        </is>
+      </c>
+      <c r="E21" s="69" t="inlineStr">
+        <is>
+          <t>------------------------</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>-----------------</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>--------------</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>---------</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>NF001</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Desktop environment with application installed</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Desktop Compatibility</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>1. Install application using Desktop zip file&lt;br&gt;2. Launch application&lt;br&gt;3. Test all major functions</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Application runs correctly on desktop environment</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>NF002</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Laptop environment with application installed</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Laptop Compatibility</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>1. Install application using Laptop zip file&lt;br&gt;2. Launch application&lt;br&gt;3. Test all major functions</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Application runs correctly on laptop environment</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>NF003</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Application is installed and launched</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Performance - Time Saving</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>1. Perform a complete diagnostic operation using the tool&lt;br&gt;2. Compare time taken with manual method</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Tool reduces testing time by approximately 80% compared to manual methods</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>NF004</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Application is installed and launched</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Usability - GUI Intuitiveness</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>1. Ask a new user to perform basic operations without instructions&lt;br&gt;2. Observe user's ability to navigate and use features</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>User can navigate and use basic features without significant confusion</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>NF005</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Application is installed and launched</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Usability - Error Handling</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>1. Deliberately perform incorrect operations&lt;br&gt;2. Observe application's response</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Application provides clear error messages and doesn't crash</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>NF006</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Application is installed and launched</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Performance - Resource Usage</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>1. Launch application&lt;br&gt;2. Monitor CPU and memory usage during operations</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Application uses reasonable system resources without excessive consumption</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>NF007</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Application is installed and launched</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Installation Process</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>1. Extract zip file to preferred location&lt;br&gt;2. Launch application by double-clicking MultiFunctionalToolApplication</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Application installs and launches without errors</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>